<commit_message>
up to round 9
</commit_message>
<xml_diff>
--- a/AFL_ML/Data/Fremantle_stats.xlsx
+++ b/AFL_ML/Data/Fremantle_stats.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:LC102"/>
+  <dimension ref="A1:LH102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="KD90" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="KJ94" activeCellId="0" sqref="KJ94"/>
@@ -1406,8 +1406,23 @@
       <c r="LB1" s="2" t="n">
         <v>10990</v>
       </c>
-      <c r="LC1" t="n">
+      <c r="LC1" s="2" t="n">
         <v>11000</v>
+      </c>
+      <c r="LD1" s="2" t="n">
+        <v>11010</v>
+      </c>
+      <c r="LE1" s="2" t="n">
+        <v>11018</v>
+      </c>
+      <c r="LF1" s="2" t="n">
+        <v>11027</v>
+      </c>
+      <c r="LG1" s="2" t="n">
+        <v>11036</v>
+      </c>
+      <c r="LH1" t="n">
+        <v>11041</v>
       </c>
     </row>
     <row r="2" ht="13.8" customHeight="1" s="3">
@@ -2355,7 +2370,22 @@
       <c r="LB2" s="2" t="n">
         <v>2023</v>
       </c>
-      <c r="LC2" t="n">
+      <c r="LC2" s="2" t="n">
+        <v>2023</v>
+      </c>
+      <c r="LD2" s="2" t="n">
+        <v>2023</v>
+      </c>
+      <c r="LE2" s="2" t="n">
+        <v>2023</v>
+      </c>
+      <c r="LF2" s="2" t="n">
+        <v>2023</v>
+      </c>
+      <c r="LG2" s="2" t="n">
+        <v>2023</v>
+      </c>
+      <c r="LH2" t="n">
         <v>2023</v>
       </c>
     </row>
@@ -3304,8 +3334,23 @@
       <c r="LB3" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="LC3" t="n">
+      <c r="LC3" s="2" t="n">
         <v>4</v>
+      </c>
+      <c r="LD3" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LE3" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="LF3" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="LG3" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="LH3" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="3">
@@ -4253,7 +4298,22 @@
       <c r="LB4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="LC4" t="n">
+      <c r="LC4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="LD4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="LE4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="LF4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="LG4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="LH4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5202,7 +5262,22 @@
       <c r="LB5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="LC5" t="n">
+      <c r="LC5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="LD5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="LE5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="LF5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="LG5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="LH5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6151,8 +6226,23 @@
       <c r="LB6" s="2" t="n">
         <v>69</v>
       </c>
-      <c r="LC6" t="n">
+      <c r="LC6" s="2" t="n">
         <v>63</v>
+      </c>
+      <c r="LD6" s="2" t="n">
+        <v>63</v>
+      </c>
+      <c r="LE6" s="2" t="n">
+        <v>68</v>
+      </c>
+      <c r="LF6" s="2" t="n">
+        <v>95</v>
+      </c>
+      <c r="LG6" s="2" t="n">
+        <v>103</v>
+      </c>
+      <c r="LH6" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="7" ht="13.8" customHeight="1" s="3">
@@ -7100,8 +7190,23 @@
       <c r="LB7" s="2" t="n">
         <v>34</v>
       </c>
-      <c r="LC7" t="n">
+      <c r="LC7" s="2" t="n">
         <v>73</v>
+      </c>
+      <c r="LD7" s="2" t="n">
+        <v>66</v>
+      </c>
+      <c r="LE7" s="2" t="n">
+        <v>105</v>
+      </c>
+      <c r="LF7" s="2" t="n">
+        <v>71</v>
+      </c>
+      <c r="LG7" s="2" t="n">
+        <v>49</v>
+      </c>
+      <c r="LH7" t="n">
+        <v>87</v>
       </c>
     </row>
     <row r="8" ht="13.8" customHeight="1" s="3">
@@ -8049,8 +8154,23 @@
       <c r="LB8" s="2" t="n">
         <v>35</v>
       </c>
-      <c r="LC8" t="n">
+      <c r="LC8" s="2" t="n">
         <v>-10</v>
+      </c>
+      <c r="LD8" s="2" t="n">
+        <v>-3</v>
+      </c>
+      <c r="LE8" s="2" t="n">
+        <v>-37</v>
+      </c>
+      <c r="LF8" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="LG8" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="LH8" t="n">
+        <v>-48</v>
       </c>
     </row>
     <row r="9" ht="13.8" customHeight="1" s="3">
@@ -8998,7 +9118,22 @@
       <c r="LB9" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="LC9" t="n">
+      <c r="LC9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="LD9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="LE9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="LF9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="LG9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="LH9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9947,8 +10082,23 @@
       <c r="LB10" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="LC10" t="n">
+      <c r="LC10" s="2" t="n">
         <v>3</v>
+      </c>
+      <c r="LD10" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="LE10" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="LF10" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="LG10" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="LH10" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" s="3">
@@ -10896,8 +11046,23 @@
       <c r="LB11" s="2" t="n">
         <v>225</v>
       </c>
-      <c r="LC11" t="n">
+      <c r="LC11" s="2" t="n">
         <v>207</v>
+      </c>
+      <c r="LD11" s="2" t="n">
+        <v>177</v>
+      </c>
+      <c r="LE11" s="2" t="n">
+        <v>194</v>
+      </c>
+      <c r="LF11" s="2" t="n">
+        <v>206</v>
+      </c>
+      <c r="LG11" s="2" t="n">
+        <v>238</v>
+      </c>
+      <c r="LH11" t="n">
+        <v>194</v>
       </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="3">
@@ -11845,8 +12010,23 @@
       <c r="LB12" s="2" t="n">
         <v>177</v>
       </c>
-      <c r="LC12" t="n">
+      <c r="LC12" s="2" t="n">
         <v>164</v>
+      </c>
+      <c r="LD12" s="2" t="n">
+        <v>159</v>
+      </c>
+      <c r="LE12" s="2" t="n">
+        <v>136</v>
+      </c>
+      <c r="LF12" s="2" t="n">
+        <v>179</v>
+      </c>
+      <c r="LG12" s="2" t="n">
+        <v>166</v>
+      </c>
+      <c r="LH12" t="n">
+        <v>175</v>
       </c>
     </row>
     <row r="13" ht="13.8" customHeight="1" s="3">
@@ -12794,8 +12974,23 @@
       <c r="LB13" s="2" t="n">
         <v>402</v>
       </c>
-      <c r="LC13" t="n">
+      <c r="LC13" s="2" t="n">
         <v>371</v>
+      </c>
+      <c r="LD13" s="2" t="n">
+        <v>336</v>
+      </c>
+      <c r="LE13" s="2" t="n">
+        <v>330</v>
+      </c>
+      <c r="LF13" s="2" t="n">
+        <v>385</v>
+      </c>
+      <c r="LG13" s="2" t="n">
+        <v>404</v>
+      </c>
+      <c r="LH13" t="n">
+        <v>369</v>
       </c>
     </row>
     <row r="14" ht="13.8" customHeight="1" s="3">
@@ -13743,8 +13938,23 @@
       <c r="LB14" s="2" t="n">
         <v>1.27</v>
       </c>
-      <c r="LC14" t="n">
+      <c r="LC14" s="2" t="n">
         <v>1.26</v>
+      </c>
+      <c r="LD14" s="2" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="LE14" s="2" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="LF14" s="2" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="LG14" s="2" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="LH14" t="n">
+        <v>1.11</v>
       </c>
     </row>
     <row r="15" ht="13.8" customHeight="1" s="3">
@@ -14692,8 +14902,23 @@
       <c r="LB15" s="2" t="n">
         <v>111</v>
       </c>
-      <c r="LC15" t="n">
+      <c r="LC15" s="2" t="n">
         <v>90</v>
+      </c>
+      <c r="LD15" s="2" t="n">
+        <v>66</v>
+      </c>
+      <c r="LE15" s="2" t="n">
+        <v>94</v>
+      </c>
+      <c r="LF15" s="2" t="n">
+        <v>91</v>
+      </c>
+      <c r="LG15" s="2" t="n">
+        <v>130</v>
+      </c>
+      <c r="LH15" t="n">
+        <v>97</v>
       </c>
     </row>
     <row r="16" ht="13.8" customHeight="1" s="3">
@@ -15641,8 +15866,23 @@
       <c r="LB16" s="2" t="n">
         <v>63</v>
       </c>
-      <c r="LC16" t="n">
+      <c r="LC16" s="2" t="n">
         <v>66</v>
+      </c>
+      <c r="LD16" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="LE16" s="2" t="n">
+        <v>49</v>
+      </c>
+      <c r="LF16" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="LG16" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="LH16" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" s="3">
@@ -16590,8 +16830,23 @@
       <c r="LB17" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="LC17" t="n">
+      <c r="LC17" s="2" t="n">
         <v>36</v>
+      </c>
+      <c r="LD17" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="LE17" s="2" t="n">
+        <v>52</v>
+      </c>
+      <c r="LF17" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="LG17" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="LH17" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="3">
@@ -17539,8 +17794,23 @@
       <c r="LB18" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="LC18" t="n">
+      <c r="LC18" s="2" t="n">
         <v>16</v>
+      </c>
+      <c r="LD18" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="LE18" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="LF18" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="LG18" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="LH18" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" s="3">
@@ -18488,8 +18758,23 @@
       <c r="LB19" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="LC19" t="n">
+      <c r="LC19" s="2" t="n">
         <v>12</v>
+      </c>
+      <c r="LD19" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="LE19" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="LF19" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="LG19" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="LH19" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" s="3">
@@ -19437,8 +19722,23 @@
       <c r="LB20" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="LC20" t="n">
+      <c r="LC20" s="2" t="n">
         <v>9</v>
+      </c>
+      <c r="LD20" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="LE20" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="LF20" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="LG20" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="LH20" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="21" ht="13.8" customHeight="1" s="3">
@@ -20386,8 +20686,23 @@
       <c r="LB21" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="LC21" t="n">
+      <c r="LC21" s="2" t="n">
         <v>3</v>
+      </c>
+      <c r="LD21" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="LE21" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="LF21" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="LG21" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="LH21" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" s="3">
@@ -21335,8 +21650,23 @@
       <c r="LB22" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="LC22" t="n">
+      <c r="LC22" s="2" t="n">
         <v>8</v>
+      </c>
+      <c r="LD22" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LE22" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="LF22" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="LG22" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="LH22" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="23" ht="13.8" customHeight="1" s="3">
@@ -22284,7 +22614,22 @@
       <c r="LB23" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="LC23" t="n">
+      <c r="LC23" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="LD23" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="LE23" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="LF23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="LG23" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="LH23" t="n">
         <v>1</v>
       </c>
     </row>
@@ -23233,8 +23578,23 @@
       <c r="LB24" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="LC24" t="n">
+      <c r="LC24" s="2" t="n">
         <v>18</v>
+      </c>
+      <c r="LD24" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="LE24" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="LF24" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="LG24" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="LH24" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" s="3">
@@ -24182,8 +24542,23 @@
       <c r="LB25" s="2" t="n">
         <v>37.5</v>
       </c>
-      <c r="LC25" t="n">
+      <c r="LC25" s="2" t="n">
         <v>50</v>
+      </c>
+      <c r="LD25" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="LE25" s="2" t="n">
+        <v>55.6</v>
+      </c>
+      <c r="LF25" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="LG25" s="2" t="n">
+        <v>53.6</v>
+      </c>
+      <c r="LH25" t="n">
+        <v>21.1</v>
       </c>
     </row>
     <row r="26" ht="13.8" customHeight="1" s="3">
@@ -25131,8 +25506,23 @@
       <c r="LB26" s="2" t="n">
         <v>44.67</v>
       </c>
-      <c r="LC26" t="n">
+      <c r="LC26" s="2" t="n">
         <v>41.22</v>
+      </c>
+      <c r="LD26" s="2" t="n">
+        <v>37.33</v>
+      </c>
+      <c r="LE26" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="LF26" s="2" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="LG26" s="2" t="n">
+        <v>26.93</v>
+      </c>
+      <c r="LH26" t="n">
+        <v>92.25</v>
       </c>
     </row>
     <row r="27" ht="13.8" customHeight="1" s="3">
@@ -26080,8 +26470,23 @@
       <c r="LB27" s="2" t="n">
         <v>16.75</v>
       </c>
-      <c r="LC27" t="n">
+      <c r="LC27" s="2" t="n">
         <v>20.61</v>
+      </c>
+      <c r="LD27" s="2" t="n">
+        <v>18.67</v>
+      </c>
+      <c r="LE27" s="2" t="n">
+        <v>18.33</v>
+      </c>
+      <c r="LF27" s="2" t="n">
+        <v>15.4</v>
+      </c>
+      <c r="LG27" s="2" t="n">
+        <v>14.43</v>
+      </c>
+      <c r="LH27" t="n">
+        <v>19.42</v>
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="3">
@@ -27029,8 +27434,23 @@
       <c r="LB28" s="2" t="n">
         <v>31</v>
       </c>
-      <c r="LC28" t="n">
+      <c r="LC28" s="2" t="n">
         <v>44</v>
+      </c>
+      <c r="LD28" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="LE28" s="2" t="n">
+        <v>42</v>
+      </c>
+      <c r="LF28" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="LG28" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="LH28" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="3">
@@ -27978,8 +28398,23 @@
       <c r="LB29" s="2" t="n">
         <v>58</v>
       </c>
-      <c r="LC29" t="n">
+      <c r="LC29" s="2" t="n">
         <v>50</v>
+      </c>
+      <c r="LD29" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="LE29" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="LF29" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="LG29" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="LH29" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="30" ht="13.8" customHeight="1" s="3">
@@ -28927,8 +29362,23 @@
       <c r="LB30" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="LC30" t="n">
+      <c r="LC30" s="2" t="n">
         <v>38</v>
+      </c>
+      <c r="LD30" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="LE30" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="LF30" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="LG30" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="LH30" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="31" ht="13.8" customHeight="1" s="3">
@@ -29876,8 +30326,23 @@
       <c r="LB31" s="2" t="n">
         <v>52</v>
       </c>
-      <c r="LC31" t="n">
+      <c r="LC31" s="2" t="n">
         <v>45</v>
+      </c>
+      <c r="LD31" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="LE31" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="LF31" s="2" t="n">
+        <v>52</v>
+      </c>
+      <c r="LG31" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="LH31" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="32" ht="13.8" customHeight="1" s="3">
@@ -30825,8 +31290,23 @@
       <c r="LB32" s="2" t="n">
         <v>2.17</v>
       </c>
-      <c r="LC32" t="n">
+      <c r="LC32" s="2" t="n">
         <v>2.5</v>
+      </c>
+      <c r="LD32" s="2" t="n">
+        <v>2.56</v>
+      </c>
+      <c r="LE32" s="2" t="n">
+        <v>2.22</v>
+      </c>
+      <c r="LF32" s="2" t="n">
+        <v>2.08</v>
+      </c>
+      <c r="LG32" s="2" t="n">
+        <v>2.11</v>
+      </c>
+      <c r="LH32" t="n">
+        <v>2.42</v>
       </c>
     </row>
     <row r="33" ht="13.8" customHeight="1" s="3">
@@ -31774,8 +32254,23 @@
       <c r="LB33" s="2" t="n">
         <v>5.78</v>
       </c>
-      <c r="LC33" t="n">
+      <c r="LC33" s="2" t="n">
         <v>5</v>
+      </c>
+      <c r="LD33" s="2" t="n">
+        <v>5.11</v>
+      </c>
+      <c r="LE33" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="LF33" s="2" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="LG33" s="2" t="n">
+        <v>3.93</v>
+      </c>
+      <c r="LH33" t="n">
+        <v>11.5</v>
       </c>
     </row>
     <row r="34" ht="13.8" customHeight="1" s="3">
@@ -32723,8 +33218,23 @@
       <c r="LB34" s="2" t="n">
         <v>40.4</v>
       </c>
-      <c r="LC34" t="n">
+      <c r="LC34" s="2" t="n">
         <v>37.8</v>
+      </c>
+      <c r="LD34" s="2" t="n">
+        <v>30.4</v>
+      </c>
+      <c r="LE34" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="LF34" s="2" t="n">
+        <v>48.1</v>
+      </c>
+      <c r="LG34" s="2" t="n">
+        <v>40.7</v>
+      </c>
+      <c r="LH34" t="n">
+        <v>39.1</v>
       </c>
     </row>
     <row r="35" ht="13.8" customHeight="1" s="3">
@@ -33672,8 +34182,23 @@
       <c r="LB35" s="2" t="n">
         <v>17.3</v>
       </c>
-      <c r="LC35" t="n">
+      <c r="LC35" s="2" t="n">
         <v>20</v>
+      </c>
+      <c r="LD35" s="2" t="n">
+        <v>19.6</v>
+      </c>
+      <c r="LE35" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="LF35" s="2" t="n">
+        <v>26.9</v>
+      </c>
+      <c r="LG35" s="2" t="n">
+        <v>25.4</v>
+      </c>
+      <c r="LH35" t="n">
+        <v>8.699999999999999</v>
       </c>
     </row>
     <row r="36" ht="13.8" customHeight="1" s="3">
@@ -34621,7 +35146,22 @@
       <c r="LB36" s="2" t="n">
         <v>188.7</v>
       </c>
-      <c r="LC36" t="n">
+      <c r="LC36" s="2" t="n">
+        <v>188.7</v>
+      </c>
+      <c r="LD36" s="2" t="n">
+        <v>189</v>
+      </c>
+      <c r="LE36" s="2" t="n">
+        <v>189.7</v>
+      </c>
+      <c r="LF36" s="2" t="n">
+        <v>189.1</v>
+      </c>
+      <c r="LG36" s="2" t="n">
+        <v>189.2</v>
+      </c>
+      <c r="LH36" t="n">
         <v>188.7</v>
       </c>
     </row>
@@ -35570,8 +36110,23 @@
       <c r="LB37" s="2" t="n">
         <v>87.3</v>
       </c>
-      <c r="LC37" t="n">
+      <c r="LC37" s="2" t="n">
         <v>87.3</v>
+      </c>
+      <c r="LD37" s="2" t="n">
+        <v>87.3</v>
+      </c>
+      <c r="LE37" s="2" t="n">
+        <v>88.3</v>
+      </c>
+      <c r="LF37" s="2" t="n">
+        <v>88.40000000000001</v>
+      </c>
+      <c r="LG37" s="2" t="n">
+        <v>88.09999999999999</v>
+      </c>
+      <c r="LH37" t="n">
+        <v>87.09999999999999</v>
       </c>
     </row>
     <row r="38" ht="13.8" customHeight="1" s="3">
@@ -36519,8 +37074,23 @@
       <c r="LB38" s="2" t="n">
         <v>25.41</v>
       </c>
-      <c r="LC38" t="n">
+      <c r="LC38" s="2" t="n">
         <v>25.41</v>
+      </c>
+      <c r="LD38" s="2" t="n">
+        <v>25.33</v>
+      </c>
+      <c r="LE38" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="LF38" s="2" t="n">
+        <v>24.66</v>
+      </c>
+      <c r="LG38" s="2" t="n">
+        <v>24.66</v>
+      </c>
+      <c r="LH38" t="n">
+        <v>24.8</v>
       </c>
     </row>
     <row r="39" ht="13.8" customHeight="1" s="3">
@@ -37468,8 +38038,23 @@
       <c r="LB39" s="2" t="n">
         <v>89.40000000000001</v>
       </c>
-      <c r="LC39" t="n">
+      <c r="LC39" s="2" t="n">
         <v>90.40000000000001</v>
+      </c>
+      <c r="LD39" s="2" t="n">
+        <v>89.59999999999999</v>
+      </c>
+      <c r="LE39" s="2" t="n">
+        <v>87</v>
+      </c>
+      <c r="LF39" s="2" t="n">
+        <v>84.09999999999999</v>
+      </c>
+      <c r="LG39" s="2" t="n">
+        <v>86.40000000000001</v>
+      </c>
+      <c r="LH39" t="n">
+        <v>86.09999999999999</v>
       </c>
     </row>
     <row r="40" ht="13.8" customHeight="1" s="3">
@@ -38417,8 +39002,23 @@
       <c r="LB40" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="LC40" t="n">
+      <c r="LC40" s="2" t="n">
         <v>7</v>
+      </c>
+      <c r="LD40" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="LE40" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="LF40" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="LG40" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="LH40" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="41" ht="13.8" customHeight="1" s="3">
@@ -39366,8 +39966,23 @@
       <c r="LB41" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="LC41" t="n">
+      <c r="LC41" s="2" t="n">
         <v>7</v>
+      </c>
+      <c r="LD41" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="LE41" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="LF41" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="LG41" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="LH41" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="42" ht="13.8" customHeight="1" s="3">
@@ -40315,8 +40930,23 @@
       <c r="LB42" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="LC42" t="n">
+      <c r="LC42" s="2" t="n">
         <v>5</v>
+      </c>
+      <c r="LD42" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LE42" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="LF42" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="LG42" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="LH42" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="43" ht="13.8" customHeight="1" s="3">
@@ -41264,7 +41894,22 @@
       <c r="LB43" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="LC43" t="n">
+      <c r="LC43" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="LD43" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="LE43" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="LF43" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="LG43" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="LH43" t="n">
         <v>4</v>
       </c>
     </row>
@@ -42213,8 +42858,23 @@
       <c r="LB44" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="LC44" t="n">
+      <c r="LC44" s="2" t="n">
         <v>130</v>
+      </c>
+      <c r="LD44" s="2" t="n">
+        <v>138</v>
+      </c>
+      <c r="LE44" s="2" t="n">
+        <v>108</v>
+      </c>
+      <c r="LF44" s="2" t="n">
+        <v>136</v>
+      </c>
+      <c r="LG44" s="2" t="n">
+        <v>111</v>
+      </c>
+      <c r="LH44" t="n">
+        <v>110</v>
       </c>
     </row>
     <row r="45" ht="13.8" customHeight="1" s="3">
@@ -43162,8 +43822,23 @@
       <c r="LB45" s="2" t="n">
         <v>277</v>
       </c>
-      <c r="LC45" t="n">
+      <c r="LC45" s="2" t="n">
         <v>235</v>
+      </c>
+      <c r="LD45" s="2" t="n">
+        <v>195</v>
+      </c>
+      <c r="LE45" s="2" t="n">
+        <v>212</v>
+      </c>
+      <c r="LF45" s="2" t="n">
+        <v>246</v>
+      </c>
+      <c r="LG45" s="2" t="n">
+        <v>280</v>
+      </c>
+      <c r="LH45" t="n">
+        <v>255</v>
       </c>
     </row>
     <row r="46" ht="13.8" customHeight="1" s="3">
@@ -44111,8 +44786,23 @@
       <c r="LB46" s="2" t="n">
         <v>313</v>
       </c>
-      <c r="LC46" t="n">
+      <c r="LC46" s="2" t="n">
         <v>283</v>
+      </c>
+      <c r="LD46" s="2" t="n">
+        <v>244</v>
+      </c>
+      <c r="LE46" s="2" t="n">
+        <v>258</v>
+      </c>
+      <c r="LF46" s="2" t="n">
+        <v>301</v>
+      </c>
+      <c r="LG46" s="2" t="n">
+        <v>312</v>
+      </c>
+      <c r="LH46" t="n">
+        <v>281</v>
       </c>
     </row>
     <row r="47" ht="13.8" customHeight="1" s="3">
@@ -45060,8 +45750,23 @@
       <c r="LB47" s="2" t="n">
         <v>77.90000000000001</v>
       </c>
-      <c r="LC47" t="n">
+      <c r="LC47" s="2" t="n">
         <v>76.3</v>
+      </c>
+      <c r="LD47" s="2" t="n">
+        <v>72.59999999999999</v>
+      </c>
+      <c r="LE47" s="2" t="n">
+        <v>78.2</v>
+      </c>
+      <c r="LF47" s="2" t="n">
+        <v>78.2</v>
+      </c>
+      <c r="LG47" s="2" t="n">
+        <v>77.2</v>
+      </c>
+      <c r="LH47" t="n">
+        <v>76.2</v>
       </c>
     </row>
     <row r="48" ht="13.8" customHeight="1" s="3">
@@ -46009,8 +46714,23 @@
       <c r="LB48" s="2" t="n">
         <v>58</v>
       </c>
-      <c r="LC48" t="n">
+      <c r="LC48" s="2" t="n">
         <v>50</v>
+      </c>
+      <c r="LD48" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="LE48" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="LF48" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="LG48" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="LH48" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="49" ht="13.8" customHeight="1" s="3">
@@ -46958,7 +47678,22 @@
       <c r="LB49" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="LC49" t="n">
+      <c r="LC49" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="LD49" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="LE49" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="LF49" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="LG49" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="LH49" t="n">
         <v>6</v>
       </c>
     </row>
@@ -47907,8 +48642,23 @@
       <c r="LB50" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="LC50" t="n">
+      <c r="LC50" s="2" t="n">
         <v>7</v>
+      </c>
+      <c r="LD50" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="LE50" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="LF50" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="LG50" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="LH50" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="51" ht="13.8" customHeight="1" s="3">
@@ -48856,8 +49606,23 @@
       <c r="LB51" s="2" t="n">
         <v>31</v>
       </c>
-      <c r="LC51" t="n">
+      <c r="LC51" s="2" t="n">
         <v>44</v>
+      </c>
+      <c r="LD51" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="LE51" s="2" t="n">
+        <v>42</v>
+      </c>
+      <c r="LF51" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="LG51" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="LH51" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="52" ht="13.8" customHeight="1" s="3">
@@ -49805,8 +50570,23 @@
       <c r="LB52" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="LC52" t="n">
+      <c r="LC52" s="2" t="n">
         <v>38</v>
+      </c>
+      <c r="LD52" s="2" t="n">
+        <v>47</v>
+      </c>
+      <c r="LE52" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="LF52" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="LG52" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="LH52" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="53" ht="13.8" customHeight="1" s="3">
@@ -50754,8 +51534,23 @@
       <c r="LB53" s="2" t="n">
         <v>44</v>
       </c>
-      <c r="LC53" t="n">
+      <c r="LC53" s="2" t="n">
         <v>43</v>
+      </c>
+      <c r="LD53" s="2" t="n">
+        <v>42</v>
+      </c>
+      <c r="LE53" s="2" t="n">
+        <v>33</v>
+      </c>
+      <c r="LF53" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="LG53" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="LH53" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="54" ht="13.8" customHeight="1" s="3">
@@ -51703,8 +52498,23 @@
       <c r="LB54" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="LC54" t="n">
+      <c r="LC54" s="2" t="n">
         <v>7</v>
+      </c>
+      <c r="LD54" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="LE54" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="LF54" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="LG54" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="LH54" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="55" ht="13.8" customHeight="1" s="3">
@@ -52652,8 +53462,23 @@
       <c r="LB55" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="LC55" t="n">
+      <c r="LC55" s="2" t="n">
         <v>3</v>
+      </c>
+      <c r="LD55" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="LE55" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="LF55" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="LG55" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="LH55" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="56" ht="13.8" customHeight="1" s="3">
@@ -53601,8 +54426,23 @@
       <c r="LB56" s="2" t="n">
         <v>77.8</v>
       </c>
-      <c r="LC56" t="n">
+      <c r="LC56" s="2" t="n">
         <v>33.3</v>
+      </c>
+      <c r="LD56" s="2" t="n">
+        <v>77.8</v>
+      </c>
+      <c r="LE56" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="LF56" s="2" t="n">
+        <v>78.59999999999999</v>
+      </c>
+      <c r="LG56" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="LH56" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="57" ht="13.8" customHeight="1" s="3">
@@ -54550,8 +55390,23 @@
       <c r="LB57" s="2" t="n">
         <v>231</v>
       </c>
-      <c r="LC57" t="n">
+      <c r="LC57" s="2" t="n">
         <v>219</v>
+      </c>
+      <c r="LD57" s="2" t="n">
+        <v>212</v>
+      </c>
+      <c r="LE57" s="2" t="n">
+        <v>204</v>
+      </c>
+      <c r="LF57" s="2" t="n">
+        <v>203</v>
+      </c>
+      <c r="LG57" s="2" t="n">
+        <v>191</v>
+      </c>
+      <c r="LH57" t="n">
+        <v>253</v>
       </c>
     </row>
     <row r="58" ht="13.8" customHeight="1" s="3">
@@ -55499,8 +56354,23 @@
       <c r="LB58" s="2" t="n">
         <v>124</v>
       </c>
-      <c r="LC58" t="n">
+      <c r="LC58" s="2" t="n">
         <v>134</v>
+      </c>
+      <c r="LD58" s="2" t="n">
+        <v>126</v>
+      </c>
+      <c r="LE58" s="2" t="n">
+        <v>113</v>
+      </c>
+      <c r="LF58" s="2" t="n">
+        <v>159</v>
+      </c>
+      <c r="LG58" s="2" t="n">
+        <v>131</v>
+      </c>
+      <c r="LH58" t="n">
+        <v>124</v>
       </c>
     </row>
     <row r="59" ht="13.8" customHeight="1" s="3">
@@ -56448,8 +57318,23 @@
       <c r="LB59" s="2" t="n">
         <v>355</v>
       </c>
-      <c r="LC59" t="n">
+      <c r="LC59" s="2" t="n">
         <v>353</v>
+      </c>
+      <c r="LD59" s="2" t="n">
+        <v>338</v>
+      </c>
+      <c r="LE59" s="2" t="n">
+        <v>317</v>
+      </c>
+      <c r="LF59" s="2" t="n">
+        <v>362</v>
+      </c>
+      <c r="LG59" s="2" t="n">
+        <v>322</v>
+      </c>
+      <c r="LH59" t="n">
+        <v>377</v>
       </c>
     </row>
     <row r="60" ht="13.8" customHeight="1" s="3">
@@ -57397,8 +58282,23 @@
       <c r="LB60" s="2" t="n">
         <v>1.86</v>
       </c>
-      <c r="LC60" t="n">
+      <c r="LC60" s="2" t="n">
         <v>1.63</v>
+      </c>
+      <c r="LD60" s="2" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="LE60" s="2" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="LF60" s="2" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="LG60" s="2" t="n">
+        <v>1.46</v>
+      </c>
+      <c r="LH60" t="n">
+        <v>2.04</v>
       </c>
     </row>
     <row r="61" ht="13.8" customHeight="1" s="3">
@@ -58346,8 +59246,23 @@
       <c r="LB61" s="2" t="n">
         <v>105</v>
       </c>
-      <c r="LC61" t="n">
+      <c r="LC61" s="2" t="n">
         <v>105</v>
+      </c>
+      <c r="LD61" s="2" t="n">
+        <v>93</v>
+      </c>
+      <c r="LE61" s="2" t="n">
+        <v>101</v>
+      </c>
+      <c r="LF61" s="2" t="n">
+        <v>99</v>
+      </c>
+      <c r="LG61" s="2" t="n">
+        <v>97</v>
+      </c>
+      <c r="LH61" t="n">
+        <v>128</v>
       </c>
     </row>
     <row r="62" ht="13.8" customHeight="1" s="3">
@@ -59295,8 +60210,23 @@
       <c r="LB62" s="2" t="n">
         <v>43</v>
       </c>
-      <c r="LC62" t="n">
+      <c r="LC62" s="2" t="n">
         <v>80</v>
+      </c>
+      <c r="LD62" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="LE62" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="LF62" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="LG62" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="LH62" t="n">
+        <v>52</v>
       </c>
     </row>
     <row r="63" ht="13.8" customHeight="1" s="3">
@@ -60244,8 +61174,23 @@
       <c r="LB63" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="LC63" t="n">
+      <c r="LC63" s="2" t="n">
         <v>39</v>
+      </c>
+      <c r="LD63" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="LE63" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="LF63" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="LG63" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="LH63" t="n">
+        <v>41</v>
       </c>
     </row>
     <row r="64" ht="13.8" customHeight="1" s="3">
@@ -61193,8 +62138,23 @@
       <c r="LB64" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="LC64" t="n">
+      <c r="LC64" s="2" t="n">
         <v>12</v>
+      </c>
+      <c r="LD64" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="LE64" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="LF64" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="LG64" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="LH64" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="65" ht="13.8" customHeight="1" s="3">
@@ -62142,8 +63102,23 @@
       <c r="LB65" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="LC65" t="n">
+      <c r="LC65" s="2" t="n">
         <v>16</v>
+      </c>
+      <c r="LD65" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="LE65" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="LF65" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="LG65" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="LH65" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="66" ht="13.8" customHeight="1" s="3">
@@ -63091,8 +64066,23 @@
       <c r="LB66" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="LC66" t="n">
+      <c r="LC66" s="2" t="n">
         <v>10</v>
+      </c>
+      <c r="LD66" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="LE66" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="LF66" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="LG66" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="LH66" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="67" ht="13.8" customHeight="1" s="3">
@@ -64040,8 +65030,23 @@
       <c r="LB67" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="LC67" t="n">
+      <c r="LC67" s="2" t="n">
         <v>5</v>
+      </c>
+      <c r="LD67" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="LE67" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="LF67" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="LG67" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LH67" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="3">
@@ -64989,8 +65994,23 @@
       <c r="LB68" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="LC68" t="n">
+      <c r="LC68" s="2" t="n">
         <v>12</v>
+      </c>
+      <c r="LD68" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="LE68" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="LF68" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="LG68" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="LH68" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="3">
@@ -65938,7 +66958,22 @@
       <c r="LB69" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="LC69" t="n">
+      <c r="LC69" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="LD69" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="LE69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="LF69" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="LG69" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="LH69" t="n">
         <v>1</v>
       </c>
     </row>
@@ -66887,8 +67922,23 @@
       <c r="LB70" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="LC70" t="n">
+      <c r="LC70" s="2" t="n">
         <v>23</v>
+      </c>
+      <c r="LD70" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="LE70" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="LF70" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="LG70" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="LH70" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="71" ht="13.8" customHeight="1" s="3">
@@ -67836,8 +68886,23 @@
       <c r="LB71" s="2" t="n">
         <v>28.6</v>
       </c>
-      <c r="LC71" t="n">
+      <c r="LC71" s="2" t="n">
         <v>43.5</v>
+      </c>
+      <c r="LD71" s="2" t="n">
+        <v>42.9</v>
+      </c>
+      <c r="LE71" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="LF71" s="2" t="n">
+        <v>47.6</v>
+      </c>
+      <c r="LG71" s="2" t="n">
+        <v>31.6</v>
+      </c>
+      <c r="LH71" t="n">
+        <v>59.1</v>
       </c>
     </row>
     <row r="72" ht="13.8" customHeight="1" s="3">
@@ -68785,8 +69850,23 @@
       <c r="LB72" s="2" t="n">
         <v>88.75</v>
       </c>
-      <c r="LC72" t="n">
+      <c r="LC72" s="2" t="n">
         <v>35.3</v>
+      </c>
+      <c r="LD72" s="2" t="n">
+        <v>37.56</v>
+      </c>
+      <c r="LE72" s="2" t="n">
+        <v>19.81</v>
+      </c>
+      <c r="LF72" s="2" t="n">
+        <v>36.2</v>
+      </c>
+      <c r="LG72" s="2" t="n">
+        <v>53.67</v>
+      </c>
+      <c r="LH72" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="73" ht="13.8" customHeight="1" s="3">
@@ -69734,8 +70814,23 @@
       <c r="LB73" s="2" t="n">
         <v>25.36</v>
       </c>
-      <c r="LC73" t="n">
+      <c r="LC73" s="2" t="n">
         <v>15.35</v>
+      </c>
+      <c r="LD73" s="2" t="n">
+        <v>16.1</v>
+      </c>
+      <c r="LE73" s="2" t="n">
+        <v>12.68</v>
+      </c>
+      <c r="LF73" s="2" t="n">
+        <v>17.24</v>
+      </c>
+      <c r="LG73" s="2" t="n">
+        <v>16.95</v>
+      </c>
+      <c r="LH73" t="n">
+        <v>17.14</v>
       </c>
     </row>
     <row r="74" ht="13.8" customHeight="1" s="3">
@@ -70683,7 +71778,22 @@
       <c r="LB74" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="LC74" t="n">
+      <c r="LC74" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="LD74" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="LE74" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="LF74" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="LG74" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="LH74" t="n">
         <v>27</v>
       </c>
     </row>
@@ -71632,8 +72742,23 @@
       <c r="LB75" s="2" t="n">
         <v>56</v>
       </c>
-      <c r="LC75" t="n">
+      <c r="LC75" s="2" t="n">
         <v>49</v>
+      </c>
+      <c r="LD75" s="2" t="n">
+        <v>49</v>
+      </c>
+      <c r="LE75" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="LF75" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="LG75" s="2" t="n">
+        <v>66</v>
+      </c>
+      <c r="LH75" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="76" ht="13.8" customHeight="1" s="3">
@@ -72581,8 +73706,23 @@
       <c r="LB76" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="LC76" t="n">
+      <c r="LC76" s="2" t="n">
         <v>36</v>
+      </c>
+      <c r="LD76" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="LE76" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="LF76" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="LG76" s="2" t="n">
+        <v>43</v>
+      </c>
+      <c r="LH76" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="77" ht="13.8" customHeight="1" s="3">
@@ -73530,8 +74670,23 @@
       <c r="LB77" s="2" t="n">
         <v>44</v>
       </c>
-      <c r="LC77" t="n">
+      <c r="LC77" s="2" t="n">
         <v>48</v>
+      </c>
+      <c r="LD77" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="LE77" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="LF77" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="LG77" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="LH77" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="78" ht="13.8" customHeight="1" s="3">
@@ -74479,8 +75634,23 @@
       <c r="LB78" s="2" t="n">
         <v>3.14</v>
       </c>
-      <c r="LC78" t="n">
+      <c r="LC78" s="2" t="n">
         <v>2.09</v>
+      </c>
+      <c r="LD78" s="2" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="LE78" s="2" t="n">
+        <v>1.92</v>
+      </c>
+      <c r="LF78" s="2" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="LG78" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="LH78" t="n">
+        <v>2.32</v>
       </c>
     </row>
     <row r="79" ht="13.8" customHeight="1" s="3">
@@ -75428,8 +76598,23 @@
       <c r="LB79" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="LC79" t="n">
+      <c r="LC79" s="2" t="n">
         <v>4.8</v>
+      </c>
+      <c r="LD79" s="2" t="n">
+        <v>6.22</v>
+      </c>
+      <c r="LE79" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="LF79" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LG79" s="2" t="n">
+        <v>6.33</v>
+      </c>
+      <c r="LH79" t="n">
+        <v>3.92</v>
       </c>
     </row>
     <row r="80" ht="13.8" customHeight="1" s="3">
@@ -76377,8 +77562,23 @@
       <c r="LB80" s="2" t="n">
         <v>27.3</v>
       </c>
-      <c r="LC80" t="n">
+      <c r="LC80" s="2" t="n">
         <v>45.8</v>
+      </c>
+      <c r="LD80" s="2" t="n">
+        <v>35.7</v>
+      </c>
+      <c r="LE80" s="2" t="n">
+        <v>52.1</v>
+      </c>
+      <c r="LF80" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="LG80" s="2" t="n">
+        <v>42.1</v>
+      </c>
+      <c r="LH80" t="n">
+        <v>41.2</v>
       </c>
     </row>
     <row r="81" ht="13.8" customHeight="1" s="3">
@@ -77326,8 +78526,23 @@
       <c r="LB81" s="2" t="n">
         <v>9.1</v>
       </c>
-      <c r="LC81" t="n">
+      <c r="LC81" s="2" t="n">
         <v>20.8</v>
+      </c>
+      <c r="LD81" s="2" t="n">
+        <v>16.1</v>
+      </c>
+      <c r="LE81" s="2" t="n">
+        <v>33.3</v>
+      </c>
+      <c r="LF81" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="LG81" s="2" t="n">
+        <v>15.8</v>
+      </c>
+      <c r="LH81" t="n">
+        <v>25.5</v>
       </c>
     </row>
     <row r="82" ht="13.8" customHeight="1" s="3">
@@ -78275,8 +79490,23 @@
       <c r="LB82" s="2" t="n">
         <v>186.9</v>
       </c>
-      <c r="LC82" t="n">
+      <c r="LC82" s="2" t="n">
         <v>187.5</v>
+      </c>
+      <c r="LD82" s="2" t="n">
+        <v>188.2</v>
+      </c>
+      <c r="LE82" s="2" t="n">
+        <v>189.7</v>
+      </c>
+      <c r="LF82" s="2" t="n">
+        <v>189</v>
+      </c>
+      <c r="LG82" s="2" t="n">
+        <v>187.2</v>
+      </c>
+      <c r="LH82" t="n">
+        <v>187.2</v>
       </c>
     </row>
     <row r="83" ht="13.8" customHeight="1" s="3">
@@ -79224,8 +80454,23 @@
       <c r="LB83" s="2" t="n">
         <v>89.40000000000001</v>
       </c>
-      <c r="LC83" t="n">
+      <c r="LC83" s="2" t="n">
         <v>86.3</v>
+      </c>
+      <c r="LD83" s="2" t="n">
+        <v>89.2</v>
+      </c>
+      <c r="LE83" s="2" t="n">
+        <v>87.59999999999999</v>
+      </c>
+      <c r="LF83" s="2" t="n">
+        <v>86.59999999999999</v>
+      </c>
+      <c r="LG83" s="2" t="n">
+        <v>85.09999999999999</v>
+      </c>
+      <c r="LH83" t="n">
+        <v>86.8</v>
       </c>
     </row>
     <row r="84" ht="13.8" customHeight="1" s="3">
@@ -80173,8 +81418,23 @@
       <c r="LB84" s="2" t="n">
         <v>25.49</v>
       </c>
-      <c r="LC84" t="n">
+      <c r="LC84" s="2" t="n">
         <v>26.8</v>
+      </c>
+      <c r="LD84" s="2" t="n">
+        <v>25.58</v>
+      </c>
+      <c r="LE84" s="2" t="n">
+        <v>25.49</v>
+      </c>
+      <c r="LF84" s="2" t="n">
+        <v>26.66</v>
+      </c>
+      <c r="LG84" s="2" t="n">
+        <v>26.41</v>
+      </c>
+      <c r="LH84" t="n">
+        <v>26.33</v>
       </c>
     </row>
     <row r="85" ht="13.8" customHeight="1" s="3">
@@ -81122,8 +82382,23 @@
       <c r="LB85" s="2" t="n">
         <v>87.8</v>
       </c>
-      <c r="LC85" t="n">
+      <c r="LC85" s="2" t="n">
         <v>92.09999999999999</v>
+      </c>
+      <c r="LD85" s="2" t="n">
+        <v>96</v>
+      </c>
+      <c r="LE85" s="2" t="n">
+        <v>99.3</v>
+      </c>
+      <c r="LF85" s="2" t="n">
+        <v>116.1</v>
+      </c>
+      <c r="LG85" s="2" t="n">
+        <v>92.2</v>
+      </c>
+      <c r="LH85" t="n">
+        <v>117.5</v>
       </c>
     </row>
     <row r="86" ht="13.8" customHeight="1" s="3">
@@ -82071,8 +83346,23 @@
       <c r="LB86" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="LC86" t="n">
+      <c r="LC86" s="2" t="n">
         <v>6</v>
+      </c>
+      <c r="LD86" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LE86" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="LF86" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="LG86" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="LH86" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="87" ht="13.8" customHeight="1" s="3">
@@ -83020,8 +84310,23 @@
       <c r="LB87" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="LC87" t="n">
+      <c r="LC87" s="2" t="n">
         <v>5</v>
+      </c>
+      <c r="LD87" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="LE87" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LF87" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="LG87" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="LH87" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="88" ht="13.8" customHeight="1" s="3">
@@ -83969,8 +85274,23 @@
       <c r="LB88" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="LC88" t="n">
+      <c r="LC88" s="2" t="n">
         <v>8</v>
+      </c>
+      <c r="LD88" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LE88" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="LF88" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LG88" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="LH88" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="89" ht="13.8" customHeight="1" s="3">
@@ -84918,8 +86238,23 @@
       <c r="LB89" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="LC89" t="n">
+      <c r="LC89" s="2" t="n">
         <v>4</v>
+      </c>
+      <c r="LD89" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="LE89" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="LF89" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="LG89" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="LH89" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="90" ht="13.8" customHeight="1" s="3">
@@ -85867,8 +87202,23 @@
       <c r="LB90" s="2" t="n">
         <v>112</v>
       </c>
-      <c r="LC90" t="n">
+      <c r="LC90" s="2" t="n">
         <v>136</v>
+      </c>
+      <c r="LD90" s="2" t="n">
+        <v>127</v>
+      </c>
+      <c r="LE90" s="2" t="n">
+        <v>132</v>
+      </c>
+      <c r="LF90" s="2" t="n">
+        <v>124</v>
+      </c>
+      <c r="LG90" s="2" t="n">
+        <v>98</v>
+      </c>
+      <c r="LH90" t="n">
+        <v>115</v>
       </c>
     </row>
     <row r="91" ht="13.8" customHeight="1" s="3">
@@ -86816,8 +88166,23 @@
       <c r="LB91" s="2" t="n">
         <v>228</v>
       </c>
-      <c r="LC91" t="n">
+      <c r="LC91" s="2" t="n">
         <v>215</v>
+      </c>
+      <c r="LD91" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="LE91" s="2" t="n">
+        <v>192</v>
+      </c>
+      <c r="LF91" s="2" t="n">
+        <v>232</v>
+      </c>
+      <c r="LG91" s="2" t="n">
+        <v>219</v>
+      </c>
+      <c r="LH91" t="n">
+        <v>246</v>
       </c>
     </row>
     <row r="92" ht="13.8" customHeight="1" s="3">
@@ -87765,8 +89130,23 @@
       <c r="LB92" s="2" t="n">
         <v>263</v>
       </c>
-      <c r="LC92" t="n">
+      <c r="LC92" s="2" t="n">
         <v>254</v>
+      </c>
+      <c r="LD92" s="2" t="n">
+        <v>255</v>
+      </c>
+      <c r="LE92" s="2" t="n">
+        <v>240</v>
+      </c>
+      <c r="LF92" s="2" t="n">
+        <v>270</v>
+      </c>
+      <c r="LG92" s="2" t="n">
+        <v>245</v>
+      </c>
+      <c r="LH92" t="n">
+        <v>294</v>
       </c>
     </row>
     <row r="93" ht="13.8" customHeight="1" s="3">
@@ -88714,8 +90094,23 @@
       <c r="LB93" s="2" t="n">
         <v>74.09999999999999</v>
       </c>
-      <c r="LC93" t="n">
+      <c r="LC93" s="2" t="n">
         <v>72</v>
+      </c>
+      <c r="LD93" s="2" t="n">
+        <v>75.40000000000001</v>
+      </c>
+      <c r="LE93" s="2" t="n">
+        <v>75.7</v>
+      </c>
+      <c r="LF93" s="2" t="n">
+        <v>74.59999999999999</v>
+      </c>
+      <c r="LG93" s="2" t="n">
+        <v>76.09999999999999</v>
+      </c>
+      <c r="LH93" t="n">
+        <v>78</v>
       </c>
     </row>
     <row r="94" ht="13.8" customHeight="1" s="3">
@@ -89663,8 +91058,23 @@
       <c r="LB94" s="2" t="n">
         <v>56</v>
       </c>
-      <c r="LC94" t="n">
+      <c r="LC94" s="2" t="n">
         <v>49</v>
+      </c>
+      <c r="LD94" s="2" t="n">
+        <v>49</v>
+      </c>
+      <c r="LE94" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="LF94" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="LG94" s="2" t="n">
+        <v>66</v>
+      </c>
+      <c r="LH94" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="95" ht="13.8" customHeight="1" s="3">
@@ -90612,8 +92022,23 @@
       <c r="LB95" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="LC95" t="n">
+      <c r="LC95" s="2" t="n">
         <v>16</v>
+      </c>
+      <c r="LD95" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="LE95" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="LF95" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="LG95" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="LH95" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="96" ht="13.8" customHeight="1" s="3">
@@ -91561,8 +92986,23 @@
       <c r="LB96" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="LC96" t="n">
+      <c r="LC96" s="2" t="n">
         <v>8</v>
+      </c>
+      <c r="LD96" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="LE96" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="LF96" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="LG96" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="LH96" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="97" ht="13.8" customHeight="1" s="3">
@@ -92510,7 +93950,22 @@
       <c r="LB97" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="LC97" t="n">
+      <c r="LC97" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="LD97" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="LE97" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="LF97" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="LG97" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="LH97" t="n">
         <v>27</v>
       </c>
     </row>
@@ -93459,8 +94914,23 @@
       <c r="LB98" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="LC98" t="n">
+      <c r="LC98" s="2" t="n">
         <v>36</v>
+      </c>
+      <c r="LD98" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="LE98" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="LF98" s="2" t="n">
+        <v>38</v>
+      </c>
+      <c r="LG98" s="2" t="n">
+        <v>43</v>
+      </c>
+      <c r="LH98" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="99" ht="13.8" customHeight="1" s="3">
@@ -94408,8 +95878,23 @@
       <c r="LB99" s="2" t="n">
         <v>45</v>
       </c>
-      <c r="LC99" t="n">
+      <c r="LC99" s="2" t="n">
         <v>41</v>
+      </c>
+      <c r="LD99" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="LE99" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="LF99" s="2" t="n">
+        <v>45</v>
+      </c>
+      <c r="LG99" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="LH99" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="100" ht="13.8" customHeight="1" s="3">
@@ -95357,7 +96842,22 @@
       <c r="LB100" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="LC100" t="n">
+      <c r="LC100" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="LD100" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="LE100" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LF100" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="LG100" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="LH100" t="n">
         <v>6</v>
       </c>
     </row>
@@ -96306,8 +97806,23 @@
       <c r="LB101" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="LC101" t="n">
+      <c r="LC101" s="2" t="n">
         <v>5</v>
+      </c>
+      <c r="LD101" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="LE101" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="LF101" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="LG101" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="LH101" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="102" ht="13.8" customHeight="1" s="3">
@@ -97255,8 +98770,23 @@
       <c r="LB102" s="2" t="n">
         <v>75</v>
       </c>
-      <c r="LC102" t="n">
+      <c r="LC102" s="2" t="n">
         <v>50</v>
+      </c>
+      <c r="LD102" s="2" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="LE102" s="2" t="n">
+        <v>43.8</v>
+      </c>
+      <c r="LF102" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="LG102" s="2" t="n">
+        <v>83.3</v>
+      </c>
+      <c r="LH102" t="n">
+        <v>84.59999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>